<commit_message>
ready T1 and T2
</commit_message>
<xml_diff>
--- a/upcoming_tournaments_T2.xlsx
+++ b/upcoming_tournaments_T2.xlsx
@@ -1239,28 +1239,28 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2025-05-29</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Scrabble</t>
+          <t>Catan</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E22" t="n">
-        <v>178</v>
+        <v>44</v>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="G22" t="n">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="H22" t="n">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1277,35 +1277,35 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-05-20</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ticket to Ride</t>
+          <t>Catan</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E23" t="n">
-        <v>114</v>
+        <v>444</v>
       </c>
       <c r="F23" t="n">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="G23" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="H23" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>free snacks and drinks</t>
+          <t>morning tournament</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-06-01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1324,19 +1324,19 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E24" t="n">
-        <v>608</v>
+        <v>56</v>
       </c>
       <c r="F24" t="n">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="G24" t="n">
-        <v>2</v>
+        <v>199</v>
       </c>
       <c r="H24" t="n">
-        <v>3</v>
+        <v>336</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1353,35 +1353,35 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ticket to Ride</t>
+          <t>Chess</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="E25" t="n">
-        <v>448</v>
+        <v>391</v>
       </c>
       <c r="F25" t="n">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="G25" t="n">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>do not bring children</t>
+          <t>meet 30 minutes before start</t>
         </is>
       </c>
     </row>
@@ -1391,35 +1391,35 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-04</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Monopoly</t>
+          <t>Scrabble</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E26" t="n">
-        <v>549</v>
+        <v>21</v>
       </c>
       <c r="F26" t="n">
-        <v>17</v>
+        <v>702</v>
       </c>
       <c r="G26" t="n">
-        <v>40</v>
+        <v>195</v>
       </c>
       <c r="H26" t="n">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>free snacks and drinks</t>
+          <t>evening tournament</t>
         </is>
       </c>
     </row>

</xml_diff>